<commit_message>
Add Decimal to Price
</commit_message>
<xml_diff>
--- a/Data/Output/Carl.xlsx
+++ b/Data/Output/Carl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Panda\Documents\UiPath\Final Project\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE12D312-151C-419E-B88D-A9247006C65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2609E844-A950-4CC7-910D-C4DB1BFE2211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="2430" windowWidth="12120" windowHeight="15555" xr2:uid="{9D382384-7E68-45AE-9DC1-E061A5703A1C}"/>
+    <workbookView xWindow="1335" yWindow="2430" windowWidth="12120" windowHeight="15555" xr2:uid="{227EF3FB-ED64-4F81-838E-A70E0B973761}"/>
   </bookViews>
   <sheets>
     <sheet name="Samsung tablet" sheetId="2" r:id="rId1"/>
@@ -52,61 +52,61 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Galaxy Tab S9+ Plus 12.4” 512GB , WiFi 6E Android Tablet, Snapdragon 8 Gen2 Processor, AMOLED Screen,S Pen, IP68 Rating, US Version,2023,Graphite</t>
+    <t>SAMSUNG Galaxy Tab S9+ Plus 12.4” 256GB , WiFi 6E Android Tablet, Snapdragon 8 Gen 2 Processor, AMOLED Screen, S Pen, Long Battery Life, IP68 Rating,US Version,2023,Beige</t>
   </si>
   <si>
     <t>4.5 out of 5 stars</t>
   </si>
   <si>
-    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToxNDI0Nzk4NzMzMjg4MDgwOjE3MTEwMTY1ODc6c3BfbXRmOjMwMDAzMjkzOTAyODYwMjo6MDo6&amp;url=%2FSAMSUNG-Android-Snapdragon-Processor-Graphite%2Fdp%2FB0C4BB67Y8%2Fref%3Dsr_1_7_sspa%3Fcrid%3DTR6ZCELH2F89%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711016587%26sprefix%3Dsams%252Caps%252C305%26sr%3D8-7-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9tdGY%26psc%3D1</t>
+    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MTo1NjIzMTI2MTE4Mjk4MDgwOjE3MTEwMjQ1OTM6c3Bfc2VhcmNoX3RoZW1hdGljOjMwMDAxOTg0MTEyODAwMjo6Mjo6&amp;url=%2FSAMSUNG-Android-Snapdragon-Processor-Battery%2Fdp%2FB0C4B92LTJ%2Fref%3Dsxin_34_pa_sp_search_thematic_sspa%3Fcontent-id%3Damzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%253Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%26crid%3D2TCNLNNT53CHD%26cv_ct_cx%3DSamsung%2Btablet%26dib%3DeyJ2IjoiMSJ9.H8IGP6LxMf_08154v6dn8UNDAiUG-IzZ4nBgpEHHsusV7Eox8qhxzh2jjalgw3pG.8fhnNTOnPIEXzWuHNeXjNSu0-XUsFRNcD9ie18YLcLI%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26pd_rd_i%3DB0C4B92LTJ%26pd_rd_r%3Dbea877a3-a3a2-4ef3-9f36-33d8075765a5%26pd_rd_w%3DaGCgT%26pd_rd_wg%3DbMBg5%26pf_rd_p%3Dd4fdc453-1595-4f7b-ba6a-eb2ac554591f%26pf_rd_r%3D883RDQQ367SZD53Y2E2E%26qid%3D1711024593%26sbo%3DRZvfv%252F%252FHxDF%252BO5021pAnSA%253D%253D%26sprefix%3Dsams%252Caps%252C328%26sr%3D1-3-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM%26psc%3D1</t>
   </si>
   <si>
     <t>Galaxy Tab S9+ Plus 12.4” 256GB , WiFi 6E Android Tablet, Snapdragon 8 Gen 2 Processor, AMOLED Screen,S Pen, IP68 Rating, US Version,2023,Graphite</t>
   </si>
   <si>
-    <t>https://www.amazon.com/SAMSUNG-Android-Snapdragon-Processor-Graphite/dp/B0C4BBNP7R/ref=sr_1_15?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-15</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy Tab S9 11” 256GB , WiFi 6E Android Tablet, Snapdragon 8 Gen 2 Processor, AMOLED Screen, S Pen, IP68 Rating, US Version, 2023, Beige</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToyMjE0OTIwODYwOTgyMDgwOjE3MTEwMTY1ODc6c3Bfc2VhcmNoX3RoZW1hdGljOjMwMDAzMjg5NjQ1MzUwMjo6Mjo6&amp;url=%2FSAMSUNG-Android-Snapdragon-Processor-Version%2Fdp%2FB0C4BBF23F%2Fref%3Dsxin_34_pa_sp_search_thematic_sspa%3Fcontent-id%3Damzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%253Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%26crid%3DTR6ZCELH2F89%26cv_ct_cx%3DSamsung%2Btablet%26dib%3DeyJ2IjoiMSJ9.H8IGP6LxMf_08154v6dn8dAOFQnpiBARnjABpeRVREcV7Eox8qhxzh2jjalgw3pG._VVeDa3NK82TZZZ4s8gxPWcxQZ3l6C3R_qBqLB7T3t0%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26pd_rd_i%3DB0C4BBF23F%26pd_rd_r%3D3cf22df9-ec8a-403f-83dd-8554010a2467%26pd_rd_w%3Dx4csL%26pd_rd_wg%3DbaDJS%26pf_rd_p%3Dd4fdc453-1595-4f7b-ba6a-eb2ac554591f%26pf_rd_r%3D98X6DHP83KZGNFNHQ1BQ%26qid%3D1711016587%26sbo%3DRZvfv%252F%252FHxDF%252BO5021pAnSA%253D%253D%26sprefix%3Dsams%252Caps%252C305%26sr%3D1-3-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM%26psc%3D1</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Tab S9 FE+ 12.4” 256GB Android Tablet, IP68 Water- and Dust-Resistant, Long Battery Life, Powerful Processor, S Pen, 8MP Camera, Lightweight Design, US Version, 2023, Silver</t>
+    <t>https://www.amazon.com/SAMSUNG-Android-Snapdragon-Processor-Graphite/dp/B0C4BBNP7R/ref=sr_1_13?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-13</t>
+  </si>
+  <si>
+    <t>Galaxy Tab S9 11” 256GB , WiFi 6E Android Tablet, Snapdragon 8 Gen 2 Processor, AMOLED Screen, S Pen, IP68 Rating, US Version, 2023, Beige</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MTo0MDY3NTcxMDY5NjM2MDgwOjE3MTEwMjQ1OTM6c3BfbXRmOjMwMDAzMjg5NjQ1MzUwMjo6MDo6&amp;url=%2FSAMSUNG-Android-Snapdragon-Processor-Version%2Fdp%2FB0C4BBF23F%2Fref%3Dsr_1_7_sspa%3Fcrid%3D2TCNLNNT53CHD%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711024593%26sprefix%3Dsams%252Caps%252C328%26sr%3D8-7-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9tdGY%26psc%3D1</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy Tab Active3 Enterprise Edition 8” Rugged Multi Purpose Tablet |64GB &amp; WiFi &amp; LTE (Unlocked) | Biometric Security (SM-T577UZKDN14), Black</t>
+  </si>
+  <si>
+    <t>4.4 out of 5 stars</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Enterprise-Unlocked-Biometric-Security-SM-T577UZKDN14/dp/B08T7RMRY9/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=2TCNLNNT53CHD&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B08T7RMRY9&amp;pd_rd_r=bea877a3-a3a2-4ef3-9f36-33d8075765a5&amp;pd_rd_w=v1296&amp;pd_rd_wg=bMBg5&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=883RDQQ367SZD53Y2E2E&amp;qid=1711024593&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C328&amp;sr=1-5-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab Active3 Enterprise Edition 8” Rugged Multi Purpose Tablet |128GB &amp; WiFi | Biometric Security (SM-T570NZKEN20), Black</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Samsung-Enterprise-Biometric-Security-SM-T570NZKEN20/dp/B08T7V27QJ/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=2TCNLNNT53CHD&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B08T7V27QJ&amp;pd_rd_r=bea877a3-a3a2-4ef3-9f36-33d8075765a5&amp;pd_rd_w=v1296&amp;pd_rd_wg=bMBg5&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=883RDQQ367SZD53Y2E2E&amp;qid=1711024593&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C328&amp;sr=1-4-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
+  </si>
+  <si>
+    <t>Galaxy Tab S9 FE Wi-Fi 10.9” 128GB, Android Tablet, IP68 Water- and Dust-Resistant, Long Battery Life, Powerful Processor, S Pen, 8MP Camera, Lightweight Design, US Version, 2023, Mint</t>
   </si>
   <si>
     <t>4.6 out of 5 stars</t>
   </si>
   <si>
-    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToyMjE0OTIwODYwOTgyMDgwOjE3MTEwMTY1ODc6c3Bfc2VhcmNoX3RoZW1hdGljOjMwMDA5MDkwMTk4MDUwMjo6MTo6&amp;url=%2FSAMSUNG-Dust-Resistant-Powerful-Processor-Lightweight%2Fdp%2FB0CCBNF8BK%2Fref%3Dsxin_34_pa_sp_search_thematic_sspa%3Fcontent-id%3Damzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%253Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%26crid%3DTR6ZCELH2F89%26cv_ct_cx%3DSamsung%2Btablet%26dib%3DeyJ2IjoiMSJ9.H8IGP6LxMf_08154v6dn8dAOFQnpiBARnjABpeRVREcV7Eox8qhxzh2jjalgw3pG._VVeDa3NK82TZZZ4s8gxPWcxQZ3l6C3R_qBqLB7T3t0%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26pd_rd_i%3DB0CCBNF8BK%26pd_rd_r%3D3cf22df9-ec8a-403f-83dd-8554010a2467%26pd_rd_w%3Dx4csL%26pd_rd_wg%3DbaDJS%26pf_rd_p%3Dd4fdc453-1595-4f7b-ba6a-eb2ac554591f%26pf_rd_r%3D98X6DHP83KZGNFNHQ1BQ%26qid%3D1711016587%26sbo%3DRZvfv%252F%252FHxDF%252BO5021pAnSA%253D%253D%26sprefix%3Dsams%252Caps%252C305%26sr%3D1-2-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM%26psc%3D1</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy Tab Active3 Enterprise Edition 8” Rugged Multi Purpose Tablet |64GB &amp; WiFi &amp; LTE (Unlocked) | Biometric Security (SM-T577UZKDN14), Black</t>
-  </si>
-  <si>
-    <t>4.4 out of 5 stars</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Enterprise-Unlocked-Biometric-Security-SM-T577UZKDN14/dp/B08T7RMRY9/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=TR6ZCELH2F89&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B08T7RMRY9&amp;pd_rd_r=3cf22df9-ec8a-403f-83dd-8554010a2467&amp;pd_rd_w=Df1mK&amp;pd_rd_wg=baDJS&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=98X6DHP83KZGNFNHQ1BQ&amp;qid=1711016587&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C305&amp;sr=1-5-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Tab Active3 Enterprise Edition 8” Rugged Multi Purpose Tablet |128GB &amp; WiFi | Biometric Security (SM-T570NZKEN20), Black</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Samsung-Enterprise-Biometric-Security-SM-T570NZKEN20/dp/B08T7V27QJ/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=TR6ZCELH2F89&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B08T7V27QJ&amp;pd_rd_r=3cf22df9-ec8a-403f-83dd-8554010a2467&amp;pd_rd_w=Df1mK&amp;pd_rd_wg=baDJS&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=98X6DHP83KZGNFNHQ1BQ&amp;qid=1711016587&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C305&amp;sr=1-4-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
-  </si>
-  <si>
-    <t>Galaxy Tab S9 FE Wi-Fi 10.9” 128GB, Android Tablet, IP68 Water- and Dust-Resistant, Long Battery Life, Powerful Processor, S Pen, 8MP Camera, Lightweight Design, US Version, 2023, Mint</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToxNDI0Nzk4NzMzMjg4MDgwOjE3MTEwMTY1ODc6c3BfYXRmOjMwMDA5MDk3NjM5MDYwMjo6MDo6&amp;url=%2FSAMSUNG-Dust-Resistant-Powerful-Processor-Lightweight%2Fdp%2FB0CCBRP9FD%2Fref%3Dsr_1_2_sspa%3Fcrid%3DTR6ZCELH2F89%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711016587%26sprefix%3Dsams%252Caps%252C305%26sr%3D8-2-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9hdGY%26psc%3D1</t>
+    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MTo0MDY3NTcxMDY5NjM2MDgwOjE3MTEwMjQ1OTM6c3BfYXRmOjMwMDA5MDk3NjM5MDYwMjo6MDo6&amp;url=%2FSAMSUNG-Dust-Resistant-Powerful-Processor-Lightweight%2Fdp%2FB0CCBRP9FD%2Fref%3Dsr_1_2_sspa%3Fcrid%3D2TCNLNNT53CHD%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711024593%26sprefix%3Dsams%252Caps%252C328%26sr%3D8-2-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9hdGY%26psc%3D1</t>
   </si>
   <si>
     <t>Galaxy Tab S9 FE Wi-Fi 10.9” 128GB Android Tablet, IP68 Water- and Dust-Resistant, Long Battery Life, Powerful Processor, S Pen, 8MP Camera, Lightweight Design, US Version, 2023, Gray</t>
   </si>
   <si>
-    <t>https://www.amazon.com/SAMSUNG-Dust-Resistant-Powerful-Processor-Lightweight/dp/B0CCX11JT6/ref=sr_1_4?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-4</t>
+    <t>https://www.amazon.com/SAMSUNG-Dust-Resistant-Powerful-Processor-Lightweight/dp/B0CCX11JT6/ref=sr_1_4?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-4</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab S9 FE Wi-Fi 10.9” 128GB, Android Tablet, IP68 Water- and Dust-Resistant, Long Battery Life, Powerful Processor, S Pen, 8MP Camera, Lightweight Design, US Version, 2023, Mint</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MTo1NjIzMTI2MTE4Mjk4MDgwOjE3MTEwMjQ1OTM6c3Bfc2VhcmNoX3RoZW1hdGljOjMwMDA5MDk3NjM5MDYwMjo6MTo6&amp;url=%2FSAMSUNG-Dust-Resistant-Powerful-Processor-Lightweight%2Fdp%2FB0CCBRP9FD%2Fref%3Dsxin_34_pa_sp_search_thematic_sspa%3Fcontent-id%3Damzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%253Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%26crid%3D2TCNLNNT53CHD%26cv_ct_cx%3DSamsung%2Btablet%26dib%3DeyJ2IjoiMSJ9.H8IGP6LxMf_08154v6dn8UNDAiUG-IzZ4nBgpEHHsusV7Eox8qhxzh2jjalgw3pG.8fhnNTOnPIEXzWuHNeXjNSu0-XUsFRNcD9ie18YLcLI%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26pd_rd_i%3DB0CCBRP9FD%26pd_rd_r%3Dbea877a3-a3a2-4ef3-9f36-33d8075765a5%26pd_rd_w%3DaGCgT%26pd_rd_wg%3DbMBg5%26pf_rd_p%3Dd4fdc453-1595-4f7b-ba6a-eb2ac554591f%26pf_rd_r%3D883RDQQ367SZD53Y2E2E%26qid%3D1711024593%26sbo%3DRZvfv%252F%252FHxDF%252BO5021pAnSA%253D%253D%26sprefix%3Dsams%252Caps%252C328%26sr%3D1-2-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM%26psc%3D1</t>
   </si>
   <si>
     <t>Galaxy Tab S6 Lite 10.4" 128GB Android Tablet, LCD Screen, S Pen Included, Slim Metal Design, AKG Dual Speakers, 8MP Rear Camera, Long Lasting Battery, US Version, 2022, Angora Blue</t>
@@ -115,55 +115,55 @@
     <t>4.7 out of 5 stars</t>
   </si>
   <si>
-    <t>https://www.amazon.com/SAMSUNG-Android-Lasting-Included-Speakers/dp/B09WYYW4TR/ref=sr_1_6?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-6</t>
+    <t>https://www.amazon.com/SAMSUNG-Android-Lasting-Included-Speakers/dp/B09WYYW4TR/ref=sr_1_6?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-6</t>
   </si>
   <si>
     <t>SAMSUNG 2020 Galaxy Tab A7 10.4’’ (2000x1200) TFT Display Wi-Fi Tablet Bundle, Qualcomm Snapdragon 662, 3GB RAM, Bluetooth, Dolby Atmos Audio, Android 10 OS w/Tigology Accessories (64GB, Gray)</t>
   </si>
   <si>
-    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToyMjE0OTIwODYwOTgyMDgwOjE3MTEwMTY1ODc6c3Bfc2VhcmNoX3RoZW1hdGljOjIwMDA5OTAwNjc1NDkxMTo6NDo6&amp;url=%2FGalaxy-Tab-A7-Snapdragon-Accessories%2Fdp%2FB08NWQGG5B%2Fref%3Dsxin_34_pa_sp_search_thematic_sspa%3Fcontent-id%3Damzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%253Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%26crid%3DTR6ZCELH2F89%26cv_ct_cx%3DSamsung%2Btablet%26dib%3DeyJ2IjoiMSJ9.H8IGP6LxMf_08154v6dn8dAOFQnpiBARnjABpeRVREcV7Eox8qhxzh2jjalgw3pG._VVeDa3NK82TZZZ4s8gxPWcxQZ3l6C3R_qBqLB7T3t0%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26pd_rd_i%3DB08NWQGG5B%26pd_rd_r%3D3cf22df9-ec8a-403f-83dd-8554010a2467%26pd_rd_w%3Dx4csL%26pd_rd_wg%3DbaDJS%26pf_rd_p%3Dd4fdc453-1595-4f7b-ba6a-eb2ac554591f%26pf_rd_r%3D98X6DHP83KZGNFNHQ1BQ%26qid%3D1711016587%26sbo%3DRZvfv%252F%252FHxDF%252BO5021pAnSA%253D%253D%26sprefix%3Dsams%252Caps%252C305%26sr%3D1-4-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM%26psc%3D1</t>
+    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MTo1NjIzMTI2MTE4Mjk4MDgwOjE3MTEwMjQ1OTM6c3Bfc2VhcmNoX3RoZW1hdGljOjIwMDA5OTAwNjc1NDkxMTo6NDo6&amp;url=%2FGalaxy-Tab-A7-Snapdragon-Accessories%2Fdp%2FB08NWQGG5B%2Fref%3Dsxin_34_pa_sp_search_thematic_sspa%3Fcontent-id%3Damzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%253Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%26crid%3D2TCNLNNT53CHD%26cv_ct_cx%3DSamsung%2Btablet%26dib%3DeyJ2IjoiMSJ9.H8IGP6LxMf_08154v6dn8UNDAiUG-IzZ4nBgpEHHsusV7Eox8qhxzh2jjalgw3pG.8fhnNTOnPIEXzWuHNeXjNSu0-XUsFRNcD9ie18YLcLI%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26pd_rd_i%3DB08NWQGG5B%26pd_rd_r%3Dbea877a3-a3a2-4ef3-9f36-33d8075765a5%26pd_rd_w%3DaGCgT%26pd_rd_wg%3DbMBg5%26pf_rd_p%3Dd4fdc453-1595-4f7b-ba6a-eb2ac554591f%26pf_rd_r%3D883RDQQ367SZD53Y2E2E%26qid%3D1711024593%26sbo%3DRZvfv%252F%252FHxDF%252BO5021pAnSA%253D%253D%26sprefix%3Dsams%252Caps%252C328%26sr%3D1-4-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM%26psc%3D1</t>
   </si>
   <si>
     <t>Galaxy Tab A8 10.5-inch Touchscreen (1920x1200) Wi-Fi Tablet Bundle, Octa-Core Processor, 3GB RAM, 32GB Memory, Bluetooth, 128GB MicroSD Card, Android 11 OS</t>
   </si>
   <si>
-    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToxNDI0Nzk4NzMzMjg4MDgwOjE3MTEwMTY1ODc6c3BfbXRmOjIwMDEwNjk2ODM2NDA5ODo6MDo6&amp;url=%2FSamsung-Galaxy-Tab-Touchscreen-Bundle%2Fdp%2FB07VN76C78%2Fref%3Dsr_1_17_sspa%3Fcrid%3DTR6ZCELH2F89%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711016587%26sprefix%3Dsams%252Caps%252C305%26sr%3D8-17-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9tdGY%26psc%3D1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Samsung-Galaxy-Tab-Touchscreen-Bundle/dp/B07VN76C78/ref=sr_1_21?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-21</t>
+    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MTo0MDY3NTcxMDY5NjM2MDgwOjE3MTEwMjQ1OTM6c3BfbXRmOjIwMDEwNjk2ODM2NDA5ODo6MDo6&amp;url=%2FSamsung-Galaxy-Tab-Touchscreen-Bundle%2Fdp%2FB07VN76C78%2Fref%3Dsr_1_17_sspa%3Fcrid%3D2TCNLNNT53CHD%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711024593%26sprefix%3Dsams%252Caps%252C328%26sr%3D8-17-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9tdGY%26psc%3D1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Samsung-Galaxy-Tab-Touchscreen-Bundle/dp/B07VN76C78/ref=sr_1_21?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-21</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy Tab S6 Lite 10.4" 64GB WiFi Android Tablet w/ S Pen Included, Slim Metal Design, Crystal Clear Display, Dual Speakers, Long Lasting Battery, SM-P610NZIAXAR, Chiffon Rose</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/SAMSUNG-Android-Included-Speakers-SM-P610NZIAXAR/dp/B086Z3QNBM/ref=sr_1_14?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-14</t>
   </si>
   <si>
     <t>Galaxy Tab A9+ Tablet 11” 128GB Android Tablet, Big Screen, Quad Speakers, Upgraded Chipset, Multi Window Display, Slim, Light, Durable Design, US Version, 2023, Graphite</t>
   </si>
   <si>
-    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToxNDI0Nzk4NzMzMjg4MDgwOjE3MTEwMTY1ODc6c3BfYXRmOjMwMDEyMDgzNjEyMjkwMjo6MDo6&amp;url=%2FSAMSUNG-Android-Speakers-Upgraded-Graphite%2Fdp%2FB0CLF2DNMV%2Fref%3Dsr_1_1_sspa%3Fcrid%3DTR6ZCELH2F89%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711016587%26sprefix%3Dsams%252Caps%252C305%26sr%3D8-1-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9hdGY%26psc%3D1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/SAMSUNG-Android-Speakers-Upgraded-Graphite/dp/B0CLF2DNMV/ref=sr_1_3?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-3</t>
+    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MTo0MDY3NTcxMDY5NjM2MDgwOjE3MTEwMjQ1OTM6c3BfYXRmOjMwMDEyMDgzNjEyMjkwMjo6MDo6&amp;url=%2FSAMSUNG-Android-Speakers-Upgraded-Graphite%2Fdp%2FB0CLF2DNMV%2Fref%3Dsr_1_1_sspa%3Fcrid%3D2TCNLNNT53CHD%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711024593%26sprefix%3Dsams%252Caps%252C328%26sr%3D8-1-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9hdGY%26psc%3D1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/SAMSUNG-Android-Speakers-Upgraded-Graphite/dp/B0CLF2DNMV/ref=sr_1_3?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-3</t>
   </si>
   <si>
     <t>SAMSUNG Galaxy Tab A9+ Tablet for Kids, 11” 128GB Android Tablet, Big Screen, Quad Speakers, Upgraded Chipset, Multi Window Display, Slim, Light, Durable Design, US Version, 2023, Silver</t>
   </si>
   <si>
-    <t>https://www.amazon.com/SAMSUNG-Android-Speakers-Upgraded-Chipset/dp/B0CLF4NVSL/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=TR6ZCELH2F89&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B0CLF4NVSL&amp;pd_rd_r=3cf22df9-ec8a-403f-83dd-8554010a2467&amp;pd_rd_w=Df1mK&amp;pd_rd_wg=baDJS&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=98X6DHP83KZGNFNHQ1BQ&amp;qid=1711016587&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C305&amp;sr=1-2-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy Tab S6 Lite 10.4" 64GB WiFi Android Tablet w/ S Pen Included, Slim Metal Design, Crystal Clear Display, Dual Speakers, Long Lasting Battery, SM-P610NZIAXAR, Chiffon Rose</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/SAMSUNG-Android-Included-Speakers-SM-P610NZIAXAR/dp/B086Z3QNBM/ref=sr_1_16?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-16</t>
+    <t>https://www.amazon.com/SAMSUNG-Android-Speakers-Upgraded-Chipset/dp/B0CLF4NVSL/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=2TCNLNNT53CHD&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B0CLF4NVSL&amp;pd_rd_r=bea877a3-a3a2-4ef3-9f36-33d8075765a5&amp;pd_rd_w=v1296&amp;pd_rd_wg=bMBg5&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=883RDQQ367SZD53Y2E2E&amp;qid=1711024593&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C328&amp;sr=1-2-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
   </si>
   <si>
     <t>SAMSUNG Galaxy Tab A9+ Tablet 11” 128GB Android Tablet, Big Screen, Quad Speakers, Upgraded Chipset, Multi Window Display, Slim, Light, Durable Design, US Version, 2023, Graphite</t>
   </si>
   <si>
-    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToyMjE0OTIwODYwOTgyMDgwOjE3MTEwMTY1ODc6c3Bfc2VhcmNoX3RoZW1hdGljOjMwMDEyMDgzNjEyMjkwMjo6MDo6&amp;url=%2FSAMSUNG-Android-Speakers-Upgraded-Graphite%2Fdp%2FB0CLF2DNMV%2Fref%3Dsxin_34_pa_sp_search_thematic_sspa%3Fcontent-id%3Damzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%253Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%26crid%3DTR6ZCELH2F89%26cv_ct_cx%3DSamsung%2Btablet%26dib%3DeyJ2IjoiMSJ9.H8IGP6LxMf_08154v6dn8dAOFQnpiBARnjABpeRVREcV7Eox8qhxzh2jjalgw3pG._VVeDa3NK82TZZZ4s8gxPWcxQZ3l6C3R_qBqLB7T3t0%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26pd_rd_i%3DB0CLF2DNMV%26pd_rd_r%3D3cf22df9-ec8a-403f-83dd-8554010a2467%26pd_rd_w%3Dx4csL%26pd_rd_wg%3DbaDJS%26pf_rd_p%3Dd4fdc453-1595-4f7b-ba6a-eb2ac554591f%26pf_rd_r%3D98X6DHP83KZGNFNHQ1BQ%26qid%3D1711016587%26sbo%3DRZvfv%252F%252FHxDF%252BO5021pAnSA%253D%253D%26sprefix%3Dsams%252Caps%252C305%26sr%3D1-1-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM%26psc%3D1</t>
+    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MTo1NjIzMTI2MTE4Mjk4MDgwOjE3MTEwMjQ1OTM6c3Bfc2VhcmNoX3RoZW1hdGljOjMwMDEyMDgzNjEyMjkwMjo6MDo6&amp;url=%2FSAMSUNG-Android-Speakers-Upgraded-Graphite%2Fdp%2FB0CLF2DNMV%2Fref%3Dsxin_34_pa_sp_search_thematic_sspa%3Fcontent-id%3Damzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%253Aamzn1.sym.d4fdc453-1595-4f7b-ba6a-eb2ac554591f%26crid%3D2TCNLNNT53CHD%26cv_ct_cx%3DSamsung%2Btablet%26dib%3DeyJ2IjoiMSJ9.H8IGP6LxMf_08154v6dn8UNDAiUG-IzZ4nBgpEHHsusV7Eox8qhxzh2jjalgw3pG.8fhnNTOnPIEXzWuHNeXjNSu0-XUsFRNcD9ie18YLcLI%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26pd_rd_i%3DB0CLF2DNMV%26pd_rd_r%3Dbea877a3-a3a2-4ef3-9f36-33d8075765a5%26pd_rd_w%3DaGCgT%26pd_rd_wg%3DbMBg5%26pf_rd_p%3Dd4fdc453-1595-4f7b-ba6a-eb2ac554591f%26pf_rd_r%3D883RDQQ367SZD53Y2E2E%26qid%3D1711024593%26sbo%3DRZvfv%252F%252FHxDF%252BO5021pAnSA%253D%253D%26sprefix%3Dsams%252Caps%252C328%26sr%3D1-1-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM%26psc%3D1</t>
   </si>
   <si>
     <t>Samsung Galaxy Tab A8 10.5-in 128GB Tablet - Gray SM-X200NZAFXAR (2022)</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Samsung-Galaxy-10-5-128GB-Tablet/dp/B09N3ZC8FL/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=TR6ZCELH2F89&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B09N3ZC8FL&amp;pd_rd_r=3cf22df9-ec8a-403f-83dd-8554010a2467&amp;pd_rd_w=Df1mK&amp;pd_rd_wg=baDJS&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=98X6DHP83KZGNFNHQ1BQ&amp;qid=1711016587&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C305&amp;sr=1-3-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
+    <t>https://www.amazon.com/Samsung-Galaxy-10-5-128GB-Tablet/dp/B09N3ZC8FL/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=2TCNLNNT53CHD&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B09N3ZC8FL&amp;pd_rd_r=bea877a3-a3a2-4ef3-9f36-33d8075765a5&amp;pd_rd_w=v1296&amp;pd_rd_wg=bMBg5&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=883RDQQ367SZD53Y2E2E&amp;qid=1711024593&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C328&amp;sr=1-3-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
   </si>
   <si>
     <t>2024 Newest Tablet Android 13 Tablets 10 Inch, Tablet 128GB ROM+16GB RAM (8+8 Virtual), 2 In 1 Tablet with keyboard, Powerful Octa-Core+13MP Camera, 1TB TF Expandable, FHD IPS Display WiFi Tablet PC</t>
@@ -172,28 +172,28 @@
     <t>4.3 out of 5 stars</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Newest-Tablet-Tablet-keyboard-Octa-Core-Expandable/dp/B0C77MDDNL/ref=sr_1_11?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-11</t>
+    <t>https://www.amazon.com/Newest-Tablet-Tablet-keyboard-Octa-Core-Expandable/dp/B0C77MDDNL/ref=sr_1_10?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-10</t>
   </si>
   <si>
     <t>Galaxy Tab A8 10.5” 64GB Android Tablet, LCD Screen, Kids Content, Smart Switch, Expandable Memory, Long Lasting Battery, Fast Charging, US Version, 2022, Silver, Amazon Exclusive</t>
   </si>
   <si>
-    <t>https://www.amazon.com/SAMSUNG-Android-Long-Lasting-Expandable-Exclusive/dp/B09N3YS882/ref=sr_1_5?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-5</t>
-  </si>
-  <si>
-    <t>Galaxy Tab A9 (64GB, 4GB, Wi-Fi Only) 8.7" Android Tablet, All Day Battery, Octa-core (6nm), Dual Speakers, International Model - X110 (256GB SD Bundle, Silver)</t>
+    <t>https://www.amazon.com/SAMSUNG-Android-Long-Lasting-Expandable-Exclusive/dp/B09N3YS882/ref=sr_1_5?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-5</t>
+  </si>
+  <si>
+    <t>Galaxy Tab A9 (64GB, 4GB, Wi-Fi Only) 8.7" Android Tablet, All Day Battery, Octa-core (6nm), Dual Speakers, International Model - X110 (256GB SD Bundle, Graphite)</t>
   </si>
   <si>
     <t>1.0 out of 5 stars</t>
   </si>
   <si>
-    <t>https://www.amazon.com/SAMSUNG-Android-Octa-core-Speakers-International/dp/B0CVYYXRRL/ref=sr_1_10?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-10</t>
+    <t>https://www.amazon.com/SAMSUNG-Android-Octa-core-Speakers-International/dp/B0CVYYM57H/ref=sr_1_19?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-19</t>
   </si>
   <si>
     <t>SAMSUNG Galaxy Tab A9+ Tablet 11” 64GB Android Tablet, Big Screen, Quad Speakers, Upgraded Chipset, Multi Window Display, Slim, Light, Durable Design, US Version, 2023, Silver</t>
   </si>
   <si>
-    <t>https://www.amazon.com/SAMSUNG-Android-Speakers-Upgraded-Chipset/dp/B0CLFH7CCV/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=TR6ZCELH2F89&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B0CLFH7CCV&amp;pd_rd_r=3cf22df9-ec8a-403f-83dd-8554010a2467&amp;pd_rd_w=Df1mK&amp;pd_rd_wg=baDJS&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=98X6DHP83KZGNFNHQ1BQ&amp;qid=1711016587&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C305&amp;sr=1-1-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
+    <t>https://www.amazon.com/SAMSUNG-Android-Speakers-Upgraded-Chipset/dp/B0CLFH7CCV/ref=sxin_12_recs_zoco_stores_brand_identity_bs?content-id=amzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811%3Aamzn1.sym.7d2e00dd-9358-4f89-aca0-04685eb73811&amp;crid=2TCNLNNT53CHD&amp;cv_ct_cx=Samsung+tablet&amp;dib=eyJ2IjoiMSJ9.TK5JheCabegjh2M4Xyks79YxQdLqnYFiilT6GwHxoP1hkbj7CrUcTKLdNVWcDlKP8zA9vh7J1iegdDqk-EnNPA.GF4BNYM4dU3Gm_z6I9BtgNyEP9ewuOswhQ9uZaW8wRY&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;pd_rd_i=B0CLFH7CCV&amp;pd_rd_r=bea877a3-a3a2-4ef3-9f36-33d8075765a5&amp;pd_rd_w=v1296&amp;pd_rd_wg=bMBg5&amp;pf_rd_p=7d2e00dd-9358-4f89-aca0-04685eb73811&amp;pf_rd_r=883RDQQ367SZD53Y2E2E&amp;qid=1711024593&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=sams%2Caps%2C328&amp;sr=1-1-5f457e4f-4cf5-45bd-948b-58563dcb013a</t>
   </si>
   <si>
     <t>Tablet 2024 Latest 10.1 Inch Android 12 Tablet with Keyboard, 8GB RAM, 256GB ROM, 1TB Expansion, 2 In 1 Octa-Core Tablet, 5G Wifi &amp; 2.4G Wifi, 6000 mAh Battery, Dual Cameras, Bluetooth/Mouse/Case/GPS</t>
@@ -202,7 +202,7 @@
     <t>4.1 out of 5 stars</t>
   </si>
   <si>
-    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToxNDI0Nzk4NzMzMjg4MDgwOjE3MTEwMTY1ODc6c3BfbXRmOjMwMDEzNTgzMjQxMzgwMjo6MDo6&amp;url=%2FAndroid-Keyboard-Expansion-Octa-Core-Bluetooth%2Fdp%2FB0CP4XT8FX%2Fref%3Dsr_1_12_sspa%3Fcrid%3DTR6ZCELH2F89%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711016587%26sprefix%3Dsams%252Caps%252C305%26sr%3D8-12-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9tdGY%26psc%3D1</t>
+    <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MTo0MDY3NTcxMDY5NjM2MDgwOjE3MTEwMjQ1OTM6c3BfbXRmOjMwMDEzNTgzMjQxMzgwMjo6MDo6&amp;url=%2FAndroid-Keyboard-Expansion-Octa-Core-Bluetooth%2Fdp%2FB0CP4XT8FX%2Fref%3Dsr_1_12_sspa%3Fcrid%3D2TCNLNNT53CHD%26dib%3DeyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI%26dib_tag%3Dse%26keywords%3DSamsung%2Btablet%26qid%3D1711024593%26sprefix%3Dsams%252Caps%252C328%26sr%3D8-12-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9tdGY%26psc%3D1</t>
   </si>
   <si>
     <t>Galaxy Tab A7 Lite (2021, 32GB, 3GB RAM) 8.7" (WiFi + Cellular) 5100mAh Battery, Android 11, 4G LTE Tablet GSM Unlocked, International Model - SM-T225 (Fast Car Charger Bundle, Gray)</t>
@@ -211,19 +211,19 @@
     <t>4.2 out of 5 stars</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Samsung-Cellular-5100mAh-Unlocked-International/dp/B0973MR9XX/ref=sr_1_18?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-18</t>
+    <t>https://www.amazon.com/Samsung-Cellular-5100mAh-Unlocked-International/dp/B0973MR9XX/ref=sr_1_15?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-15</t>
   </si>
   <si>
     <t>SAMSUNG SM-T290NZKAXAR, Galaxy Tab A 8.0" 32 GB Wifi Android 9.0 Pie Tablet Black 2019</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Samsung-Galaxy-Android-Tablet-Black/dp/B07VDB92RK/ref=sr_1_20?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-20</t>
+    <t>https://www.amazon.com/Samsung-Galaxy-Android-Tablet-Black/dp/B07VDB92RK/ref=sr_1_20?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-20</t>
   </si>
   <si>
     <t>Tab M9-2023 - Tablet - Long Battery Life - 9" HD - Front 2MP &amp; Rear 8MP Camera - 3GB Memory - 32GB Storage - Android 12 or Later - Folio Case Included,Gray</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Lenovo-Tab-M9-2023-Battery-Included/dp/B0BYPHZWZK/ref=sr_1_13?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-13</t>
+    <t>https://www.amazon.com/Lenovo-Tab-M9-2023-Battery-Included/dp/B0BYPHZWZK/ref=sr_1_11?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-11</t>
   </si>
   <si>
     <t>Galaxy Tab A 8.0 T387A 32GB Unlocked AT&amp;T Tablet - Black</t>
@@ -232,13 +232,13 @@
     <t>3.9 out of 5 stars</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Samsung-Galaxy-T387A-Unlocked-Tablet/dp/B07XDM26Z3/ref=sr_1_14?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-14</t>
+    <t>https://www.amazon.com/Samsung-Galaxy-T387A-Unlocked-Tablet/dp/B07XDM26Z3/ref=sr_1_16?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-16</t>
   </si>
   <si>
     <t>SAMSUNG Galaxy Tab A7 Lite 8.7" 32GB WiFi Android Tablet, Compact, Portable, Slim Design, Kid Friendly, Sturdy Metal Frame, Expandable Storage, Long Lasting Battery, US Version, 2021, Silver</t>
   </si>
   <si>
-    <t>https://www.amazon.com/SAMSUNG-Android-Compact-Lasting-Battery/dp/B094PXZMP6/ref=sr_1_8?crid=TR6ZCELH2F89&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOoIDpU9q8snFDiQrnivuQH4oiDKmO9TSRMspjwQoQC3FCyMDng1OqBoV0Z1txGFFuJpGFPe_ZiXALcX1eGDWwUdwwnI5dX7MIl0-b960ewB3eStmR-pV_6kJWHmkjaEuvHjtG_tjzpzP9Dsq-GtlVoM.yjhQArGSahUDokrAJ3Z7IyfB57TGcwKDvJewCi_gtoU&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711016587&amp;sprefix=sams%2Caps%2C305&amp;sr=8-8</t>
+    <t>https://www.amazon.com/SAMSUNG-Android-Compact-Lasting-Battery/dp/B094PXZMP6/ref=sr_1_8?crid=2TCNLNNT53CHD&amp;dib=eyJ2IjoiMSJ9.jJO6Tdz4qWTToEKLv-21nMlRhZRnnIV14CeGv30l2dY6v-R8Cd3-iJlXZSzuifM-DGMFIF_S5ym-b8SN2mOsOl2hXg9AWBVFsqY5U-t9Y9TfF9lxUIJ4OKlb-wwzu6sxFF-FM54pEDc98gtFnxWlZ3KoxStnUPM071Nu9FSGW76wDZsAu6SwyxF7H8TETdX2z5RuFCH6fM6FOf0LUWFxR3jtG_tjzpzP9Dsq-GtlVoM.pU-9Fqm61UgkIuv8I9r2PkOvxfFujI4mEQtq-FhsYdI&amp;dib_tag=se&amp;keywords=Samsung+tablet&amp;qid=1711024593&amp;sprefix=sams%2Caps%2C328&amp;sr=8-8</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1B8907-01C3-4310-98B0-20813031D1D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F1B8DB-8A5B-4FF2-881C-3E40F2996FD7}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -624,7 +624,7 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="188" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -648,69 +648,69 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1">
-        <v>951</v>
+        <v>899</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>898</v>
+        <v>898.49</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>796</v>
+        <v>796.19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>599</v>
+        <v>569.99</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1">
-        <v>476</v>
+        <v>291</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -721,98 +721,98 @@
         <v>15</v>
       </c>
       <c r="B6" s="1">
-        <v>569</v>
+        <v>441.85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>291</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>349.99</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1">
-        <v>441</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="1">
-        <v>291</v>
+        <v>478</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="1">
-        <v>349</v>
+        <v>349.99</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="1">
-        <v>349</v>
+        <v>349.99</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="1">
-        <v>291</v>
+        <v>291.99</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="1">
-        <v>7021</v>
+        <v>7032</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="1">
-        <v>268</v>
+        <v>268.98</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1">
-        <v>1859</v>
+        <v>1860</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -829,13 +829,13 @@
         <v>6</v>
       </c>
       <c r="D12" s="1">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -846,75 +846,75 @@
         <v>6</v>
       </c>
       <c r="D13" s="1">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="1">
-        <v>219</v>
+        <v>224.49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1">
-        <v>442</v>
+        <v>18146</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1">
-        <v>219</v>
+        <v>219.99</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1">
-        <v>442</v>
+        <v>458</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="B16" s="1">
-        <v>219</v>
+        <v>219.99</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="1">
-        <v>442</v>
+        <v>458</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="1">
-        <v>219</v>
+        <v>219.99</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1">
-        <v>18145</v>
+        <v>458</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>38</v>
@@ -925,13 +925,13 @@
         <v>39</v>
       </c>
       <c r="B18" s="1">
-        <v>219</v>
+        <v>219.99</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="1">
-        <v>442</v>
+        <v>458</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>40</v>
@@ -948,52 +948,52 @@
         <v>6</v>
       </c>
       <c r="D19" s="1">
-        <v>23026</v>
+        <v>23049</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="1">
-        <v>199</v>
+        <v>199.98</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="1">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="1">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="1">
-        <v>23026</v>
+        <v>23049</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="1">
-        <v>179</v>
+        <v>172.49</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>49</v>
@@ -1010,13 +1010,13 @@
         <v>51</v>
       </c>
       <c r="B23" s="1">
-        <v>169</v>
+        <v>169.99</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>442</v>
+        <v>458</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>52</v>
@@ -1027,7 +1027,7 @@
         <v>53</v>
       </c>
       <c r="B24" s="1">
-        <v>169</v>
+        <v>169.99</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>54</v>
@@ -1039,7 +1039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
@@ -1056,15 +1056,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="1">
-        <v>148</v>
+        <v>148.12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D26" s="1">
         <v>10341</v>
@@ -1073,15 +1073,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B27" s="1">
-        <v>99</v>
+        <v>99.99</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D27" s="1">
         <v>657</v>
@@ -1090,12 +1090,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="1">
-        <v>94</v>
+        <v>94.99</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>64</v>
@@ -1107,7 +1107,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>6</v>
       </c>
       <c r="D29" s="1">
-        <v>3977</v>
+        <v>3978</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>67</v>
@@ -1127,7 +1127,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC6A80D-95F4-4031-862C-D16DA029CE76}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB09FAC8-7842-4805-A800-58A60A55CAE7}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>